<commit_message>
Add Batik 1.12 (the version is just an educated guess)
</commit_message>
<xml_diff>
--- a/doc-project/R2019b jarext worksheet.xlsx
+++ b/doc-project/R2019b jarext worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janke/local/repos/matlab-jump/doc-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC57A34-3666-B64E-8601-4FE6A2A977BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9729EE34-FB20-F14B-92BD-F44F78D98FB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33820" windowHeight="25560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29940" windowHeight="25360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="R2019b" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="566">
   <si>
     <t>Title</t>
   </si>
@@ -1722,6 +1722,15 @@
   </si>
   <si>
     <t>TMate Open Source License</t>
+  </si>
+  <si>
+    <t>Total OSS</t>
+  </si>
+  <si>
+    <t>OSS+Valid</t>
+  </si>
+  <si>
+    <t>Not needed. These XML things ship with JDK itself starting with 1.8. Though maybe we _should_ include them to induce Matlab-congruent failure states.</t>
   </si>
 </sst>
 </file>
@@ -1739,26 +1748,31 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2047,13 +2061,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L194"/>
+  <dimension ref="A1:M195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K167" sqref="K167"/>
+      <selection pane="bottomRight" activeCell="K28" sqref="K28:K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2066,11 +2080,12 @@
     <col min="6" max="6" width="18.1640625" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
     <col min="8" max="8" width="28.83203125" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" customWidth="1"/>
-    <col min="11" max="11" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" customWidth="1"/>
+    <col min="11" max="11" width="8.1640625" customWidth="1"/>
+    <col min="12" max="12" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2099,16 +2114,19 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="5"/>
@@ -2122,11 +2140,14 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="L2" s="10" t="s">
+      <c r="J2" s="5">
+        <v>1</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -2155,9 +2176,12 @@
       <c r="J3" s="5">
         <v>1</v>
       </c>
-      <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K3" s="5">
+        <v>1</v>
+      </c>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="5"/>
@@ -2171,8 +2195,11 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="5"/>
@@ -2186,8 +2213,11 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="5"/>
@@ -2199,8 +2229,11 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="5"/>
@@ -2212,8 +2245,11 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="12" t="s">
@@ -2229,11 +2265,14 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="L8" s="10" t="s">
+      <c r="J8" s="5">
+        <v>1</v>
+      </c>
+      <c r="M8" s="10" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="5"/>
@@ -2247,8 +2286,11 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="5"/>
@@ -2262,8 +2304,11 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
@@ -2292,8 +2337,11 @@
       <c r="J11" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -2322,8 +2370,11 @@
       <c r="J12" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>25</v>
       </c>
@@ -2352,8 +2403,11 @@
       <c r="J13" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>30</v>
       </c>
@@ -2382,9 +2436,12 @@
       <c r="J14" s="5">
         <v>1</v>
       </c>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K14" s="5">
+        <v>1</v>
+      </c>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
@@ -2413,8 +2470,11 @@
       <c r="J15" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
@@ -2443,8 +2503,11 @@
       <c r="J16" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>45</v>
       </c>
@@ -2473,8 +2536,11 @@
       <c r="J17" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K17" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>50</v>
       </c>
@@ -2503,8 +2569,11 @@
       <c r="J18" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>53</v>
       </c>
@@ -2533,8 +2602,11 @@
       <c r="J19" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>55</v>
       </c>
@@ -2563,8 +2635,11 @@
       <c r="J20" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>57</v>
       </c>
@@ -2593,8 +2668,11 @@
       <c r="J21" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>59</v>
       </c>
@@ -2623,8 +2701,11 @@
       <c r="J22" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>63</v>
       </c>
@@ -2653,8 +2734,11 @@
       <c r="J23" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>67</v>
       </c>
@@ -2683,9 +2767,12 @@
       <c r="J24" s="5">
         <v>1</v>
       </c>
-      <c r="K24" s="5"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K24" s="5">
+        <v>1</v>
+      </c>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>71</v>
       </c>
@@ -2714,8 +2801,11 @@
       <c r="J25" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K25" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>76</v>
       </c>
@@ -2744,9 +2834,12 @@
       <c r="J26" s="5">
         <v>1</v>
       </c>
-      <c r="K26" s="5"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K26" s="5">
+        <v>1</v>
+      </c>
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>81</v>
       </c>
@@ -2775,9 +2868,12 @@
       <c r="J27" s="5">
         <v>1</v>
       </c>
-      <c r="K27" s="5"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K27" s="5">
+        <v>1</v>
+      </c>
+      <c r="L27" s="5"/>
+    </row>
+    <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>87</v>
       </c>
@@ -2799,11 +2895,17 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-      <c r="L28" s="10" t="s">
+      <c r="J28" s="5">
+        <v>1</v>
+      </c>
+      <c r="K28" s="5">
+        <v>1</v>
+      </c>
+      <c r="M28" s="10" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>91</v>
       </c>
@@ -2825,11 +2927,17 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-      <c r="L29" s="10" t="s">
+      <c r="J29" s="5">
+        <v>1</v>
+      </c>
+      <c r="K29" s="5">
+        <v>1</v>
+      </c>
+      <c r="M29" s="10" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>93</v>
       </c>
@@ -2851,8 +2959,14 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J30" s="5">
+        <v>1</v>
+      </c>
+      <c r="K30" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>95</v>
       </c>
@@ -2874,8 +2988,14 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J31" s="5">
+        <v>1</v>
+      </c>
+      <c r="K31" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>97</v>
       </c>
@@ -2897,8 +3017,14 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J32" s="5">
+        <v>1</v>
+      </c>
+      <c r="K32" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>99</v>
       </c>
@@ -2920,8 +3046,14 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J33" s="5">
+        <v>1</v>
+      </c>
+      <c r="K33" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>101</v>
       </c>
@@ -2943,8 +3075,14 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J34" s="5">
+        <v>1</v>
+      </c>
+      <c r="K34" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>103</v>
       </c>
@@ -2966,8 +3104,14 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J35" s="5">
+        <v>1</v>
+      </c>
+      <c r="K35" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>105</v>
       </c>
@@ -2989,8 +3133,14 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J36" s="5">
+        <v>1</v>
+      </c>
+      <c r="K36" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>107</v>
       </c>
@@ -3012,8 +3162,14 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J37" s="5">
+        <v>1</v>
+      </c>
+      <c r="K37" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>109</v>
       </c>
@@ -3035,8 +3191,14 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J38" s="5">
+        <v>1</v>
+      </c>
+      <c r="K38" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>111</v>
       </c>
@@ -3058,8 +3220,14 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J39" s="5">
+        <v>1</v>
+      </c>
+      <c r="K39" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>113</v>
       </c>
@@ -3081,8 +3249,14 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J40" s="5">
+        <v>1</v>
+      </c>
+      <c r="K40" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>115</v>
       </c>
@@ -3104,8 +3278,14 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J41" s="5">
+        <v>1</v>
+      </c>
+      <c r="K41" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>117</v>
       </c>
@@ -3127,8 +3307,14 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J42" s="5">
+        <v>1</v>
+      </c>
+      <c r="K42" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>119</v>
       </c>
@@ -3150,8 +3336,14 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J43" s="5">
+        <v>1</v>
+      </c>
+      <c r="K43" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>121</v>
       </c>
@@ -3173,8 +3365,14 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J44" s="5">
+        <v>1</v>
+      </c>
+      <c r="K44" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>123</v>
       </c>
@@ -3196,8 +3394,14 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J45" s="5">
+        <v>1</v>
+      </c>
+      <c r="K45" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="12" t="s">
@@ -3215,11 +3419,17 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
-      <c r="L46" s="10" t="s">
+      <c r="J46" s="5">
+        <v>1</v>
+      </c>
+      <c r="K46" s="5">
+        <v>1</v>
+      </c>
+      <c r="M46" s="10" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="12" t="s">
@@ -3237,11 +3447,17 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
-      <c r="L47" s="10" t="s">
+      <c r="J47" s="5">
+        <v>1</v>
+      </c>
+      <c r="K47" s="5">
+        <v>1</v>
+      </c>
+      <c r="M47" s="10" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>128</v>
       </c>
@@ -3270,8 +3486,11 @@
       <c r="J48" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K48" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>131</v>
       </c>
@@ -3300,8 +3519,11 @@
       <c r="J49" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K49" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>134</v>
       </c>
@@ -3322,11 +3544,14 @@
       <c r="J50" s="5">
         <v>1</v>
       </c>
-      <c r="L50" t="s">
+      <c r="K50" s="5">
+        <v>1</v>
+      </c>
+      <c r="M50" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>137</v>
       </c>
@@ -3355,8 +3580,11 @@
       <c r="J51" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K51" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>141</v>
       </c>
@@ -3385,8 +3613,11 @@
       <c r="J52" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K52" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>146</v>
       </c>
@@ -3415,8 +3646,11 @@
       <c r="J53" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K53" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>150</v>
       </c>
@@ -3445,8 +3679,11 @@
       <c r="J54" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K54" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>153</v>
       </c>
@@ -3475,8 +3712,11 @@
       <c r="J55" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K55" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>156</v>
       </c>
@@ -3499,11 +3739,14 @@
       <c r="J56" s="5">
         <v>1</v>
       </c>
-      <c r="L56" t="s">
+      <c r="K56" s="5">
+        <v>1</v>
+      </c>
+      <c r="M56" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="5"/>
@@ -3517,8 +3760,11 @@
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J57" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="5"/>
@@ -3532,8 +3778,11 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J58" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="5"/>
@@ -3547,8 +3796,11 @@
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J59" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="5"/>
@@ -3562,8 +3814,11 @@
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J60" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="5"/>
@@ -3577,8 +3832,11 @@
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J61" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="5"/>
@@ -3592,8 +3850,11 @@
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J62" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="5"/>
@@ -3607,8 +3868,11 @@
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J63" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="5"/>
@@ -3622,8 +3886,11 @@
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J64" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="5"/>
@@ -3637,8 +3904,11 @@
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J65" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>167</v>
       </c>
@@ -3667,12 +3937,15 @@
       <c r="J66" s="5">
         <v>1</v>
       </c>
-      <c r="K66" s="5"/>
-      <c r="L66" s="5" t="s">
+      <c r="K66" s="5">
+        <v>1</v>
+      </c>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="5"/>
@@ -3686,11 +3959,14 @@
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
-      <c r="L67" s="10" t="s">
+      <c r="J67" s="5">
+        <v>1</v>
+      </c>
+      <c r="M67" s="10" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="5"/>
@@ -3702,8 +3978,11 @@
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J68" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="5"/>
@@ -3715,8 +3994,11 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J69" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>176</v>
       </c>
@@ -3745,11 +4027,14 @@
       <c r="J70" s="5">
         <v>1</v>
       </c>
-      <c r="L70" s="5" t="s">
+      <c r="K70" s="5">
+        <v>1</v>
+      </c>
+      <c r="M70" s="5" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>181</v>
       </c>
@@ -3775,14 +4060,17 @@
       <c r="I71" s="3">
         <v>2.4</v>
       </c>
-      <c r="J71">
-        <v>1</v>
-      </c>
-      <c r="L71" s="10" t="s">
+      <c r="J71" s="5">
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <v>1</v>
+      </c>
+      <c r="M71" s="10" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="5"/>
@@ -3802,14 +4090,17 @@
       <c r="I72" s="3">
         <v>2.4</v>
       </c>
-      <c r="J72">
-        <v>1</v>
-      </c>
-      <c r="L72" s="10" t="s">
+      <c r="J72" s="5">
+        <v>1</v>
+      </c>
+      <c r="K72">
+        <v>1</v>
+      </c>
+      <c r="M72" s="10" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="5"/>
@@ -3823,11 +4114,14 @@
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
-      <c r="L73" s="10" t="s">
+      <c r="J73" s="5">
+        <v>1</v>
+      </c>
+      <c r="M73" s="10" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>187</v>
       </c>
@@ -3843,8 +4137,11 @@
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J74" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>190</v>
       </c>
@@ -3862,8 +4159,11 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J75" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>194</v>
       </c>
@@ -3892,10 +4192,13 @@
       <c r="J76" s="5">
         <v>1</v>
       </c>
-      <c r="K76" s="5"/>
+      <c r="K76" s="5">
+        <v>1</v>
+      </c>
       <c r="L76" s="5"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M76" s="5"/>
+    </row>
+    <row r="77" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>199</v>
       </c>
@@ -3924,9 +4227,12 @@
       <c r="J77" s="5">
         <v>1</v>
       </c>
-      <c r="K77" s="5"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K77" s="5">
+        <v>1</v>
+      </c>
+      <c r="L77" s="5"/>
+    </row>
+    <row r="78" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>205</v>
       </c>
@@ -3955,9 +4261,12 @@
       <c r="J78" s="5">
         <v>1</v>
       </c>
-      <c r="K78" s="5"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K78" s="5">
+        <v>1</v>
+      </c>
+      <c r="L78" s="5"/>
+    </row>
+    <row r="79" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
         <v>207</v>
       </c>
@@ -3986,9 +4295,12 @@
       <c r="J79" s="5">
         <v>1</v>
       </c>
-      <c r="K79" s="5"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K79" s="5">
+        <v>1</v>
+      </c>
+      <c r="L79" s="5"/>
+    </row>
+    <row r="80" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>212</v>
       </c>
@@ -4017,9 +4329,12 @@
       <c r="J80" s="5">
         <v>1</v>
       </c>
-      <c r="K80" s="5"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K80" s="5">
+        <v>1</v>
+      </c>
+      <c r="L80" s="5"/>
+    </row>
+    <row r="81" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="12" t="s">
@@ -4033,8 +4348,11 @@
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J81" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="5"/>
@@ -4046,8 +4364,11 @@
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J82" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="5"/>
@@ -4061,11 +4382,14 @@
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
-      <c r="L83" s="10" t="s">
+      <c r="J83" s="5">
+        <v>1</v>
+      </c>
+      <c r="M83" s="10" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="5"/>
@@ -4079,11 +4403,14 @@
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
-      <c r="L84" s="10" t="s">
+      <c r="J84" s="5">
+        <v>1</v>
+      </c>
+      <c r="M84" s="10" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="5"/>
@@ -4097,11 +4424,14 @@
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
-      <c r="L85" s="10" t="s">
+      <c r="J85" s="5">
+        <v>1</v>
+      </c>
+      <c r="M85" s="10" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="5"/>
@@ -4115,8 +4445,11 @@
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J86" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="5"/>
@@ -4130,8 +4463,11 @@
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J87" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="5"/>
@@ -4145,8 +4481,11 @@
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J88" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="5"/>
@@ -4160,8 +4499,11 @@
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J89" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="5"/>
@@ -4175,8 +4517,11 @@
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J90" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="5"/>
@@ -4190,8 +4535,11 @@
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J91" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="5"/>
@@ -4205,8 +4553,11 @@
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J92" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="5"/>
@@ -4218,11 +4569,14 @@
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
-      <c r="L93" s="10" t="s">
+      <c r="J93" s="5">
+        <v>1</v>
+      </c>
+      <c r="M93" s="10" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>228</v>
       </c>
@@ -4249,8 +4603,11 @@
       <c r="J94" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K94" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>234</v>
       </c>
@@ -4277,8 +4634,11 @@
       <c r="J95" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K95" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>237</v>
       </c>
@@ -4305,8 +4665,11 @@
       <c r="J96" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K96" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>239</v>
       </c>
@@ -4333,8 +4696,11 @@
       <c r="J97" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K97" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
         <v>243</v>
       </c>
@@ -4361,8 +4727,11 @@
       <c r="J98" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K98" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>246</v>
       </c>
@@ -4389,8 +4758,11 @@
       <c r="J99" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K99" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
         <v>250</v>
       </c>
@@ -4419,9 +4791,12 @@
       <c r="J100" s="5">
         <v>1</v>
       </c>
-      <c r="K100" s="5"/>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K100" s="5">
+        <v>1</v>
+      </c>
+      <c r="L100" s="5"/>
+    </row>
+    <row r="101" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>254</v>
       </c>
@@ -4450,9 +4825,12 @@
       <c r="J101" s="5">
         <v>1</v>
       </c>
-      <c r="K101" s="5"/>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K101" s="5">
+        <v>1</v>
+      </c>
+      <c r="L101" s="5"/>
+    </row>
+    <row r="102" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="5"/>
@@ -4464,11 +4842,14 @@
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
-      <c r="L102" s="10" t="s">
+      <c r="J102" s="5">
+        <v>1</v>
+      </c>
+      <c r="M102" s="10" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
         <v>259</v>
       </c>
@@ -4497,9 +4878,12 @@
       <c r="J103" s="5">
         <v>1</v>
       </c>
-      <c r="K103" s="5"/>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K103" s="5">
+        <v>1</v>
+      </c>
+      <c r="L103" s="5"/>
+    </row>
+    <row r="104" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
         <v>261</v>
       </c>
@@ -4528,9 +4912,12 @@
       <c r="J104" s="5">
         <v>1</v>
       </c>
-      <c r="K104" s="5"/>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K104" s="5">
+        <v>1</v>
+      </c>
+      <c r="L104" s="5"/>
+    </row>
+    <row r="105" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
         <v>261</v>
       </c>
@@ -4559,9 +4946,12 @@
       <c r="J105" s="5">
         <v>1</v>
       </c>
-      <c r="K105" s="5"/>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K105" s="5">
+        <v>1</v>
+      </c>
+      <c r="L105" s="5"/>
+    </row>
+    <row r="106" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
         <v>268</v>
       </c>
@@ -4579,11 +4969,14 @@
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
-      <c r="L106" s="10" t="s">
+      <c r="J106" s="5">
+        <v>1</v>
+      </c>
+      <c r="M106" s="10" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>272</v>
       </c>
@@ -4601,8 +4994,11 @@
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J107" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="3"/>
       <c r="B108" s="5" t="s">
         <v>275</v>
@@ -4620,11 +5016,14 @@
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
-      <c r="L108" s="10" t="s">
+      <c r="J108" s="5">
+        <v>0</v>
+      </c>
+      <c r="M108" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="3"/>
       <c r="B109" s="5" t="s">
         <v>275</v>
@@ -4642,11 +5041,14 @@
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
-      <c r="L109" s="10" t="s">
+      <c r="J109" s="5">
+        <v>0</v>
+      </c>
+      <c r="M109" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="12" t="s">
@@ -4660,8 +5062,11 @@
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J110" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A111" s="3"/>
       <c r="B111" s="5" t="s">
         <v>275</v>
@@ -4679,11 +5084,14 @@
       <c r="G111" s="3"/>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
-      <c r="L111" s="10" t="s">
+      <c r="J111" s="5">
+        <v>0</v>
+      </c>
+      <c r="M111" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A112" s="3"/>
       <c r="B112" s="5" t="s">
         <v>275</v>
@@ -4701,11 +5109,14 @@
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
-      <c r="L112" s="10" t="s">
+      <c r="J112" s="5">
+        <v>0</v>
+      </c>
+      <c r="M112" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A113" s="3"/>
       <c r="B113" s="5" t="s">
         <v>275</v>
@@ -4723,11 +5134,14 @@
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
-      <c r="L113" s="10" t="s">
+      <c r="J113" s="5">
+        <v>0</v>
+      </c>
+      <c r="M113" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A114" s="3"/>
       <c r="B114" s="5" t="s">
         <v>275</v>
@@ -4745,11 +5159,14 @@
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
-      <c r="L114" s="10" t="s">
+      <c r="J114" s="5">
+        <v>0</v>
+      </c>
+      <c r="M114" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="12" t="s">
@@ -4763,11 +5180,14 @@
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
-      <c r="L115" s="10" t="s">
+      <c r="J115" s="5">
+        <v>0</v>
+      </c>
+      <c r="M115" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A116" s="3"/>
       <c r="B116" s="5" t="s">
         <v>275</v>
@@ -4785,11 +5205,14 @@
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
-      <c r="L116" s="10" t="s">
+      <c r="J116" s="5">
+        <v>0</v>
+      </c>
+      <c r="M116" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
         <v>286</v>
       </c>
@@ -4815,15 +5238,18 @@
       <c r="I117" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="J117">
-        <v>1</v>
-      </c>
-      <c r="K117" s="12"/>
-      <c r="L117" s="12" t="s">
+      <c r="J117" s="5">
+        <v>1</v>
+      </c>
+      <c r="K117">
+        <v>1</v>
+      </c>
+      <c r="L117" s="12"/>
+      <c r="M117" s="12" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="12" t="s">
@@ -4847,14 +5273,17 @@
       <c r="I118" s="12" t="s">
         <v>526</v>
       </c>
-      <c r="J118">
-        <v>1</v>
-      </c>
-      <c r="L118" s="10" t="s">
+      <c r="J118" s="5">
+        <v>1</v>
+      </c>
+      <c r="K118">
+        <v>1</v>
+      </c>
+      <c r="M118" s="10" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="12" t="s">
@@ -4878,14 +5307,17 @@
       <c r="I119" s="12" t="s">
         <v>538</v>
       </c>
-      <c r="J119">
-        <v>1</v>
-      </c>
-      <c r="L119" s="10" t="s">
+      <c r="J119" s="5">
+        <v>1</v>
+      </c>
+      <c r="K119">
+        <v>1</v>
+      </c>
+      <c r="M119" s="10" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="12" t="s">
@@ -4909,14 +5341,17 @@
       <c r="I120" s="12" t="s">
         <v>538</v>
       </c>
-      <c r="J120">
-        <v>1</v>
-      </c>
-      <c r="L120" s="12" t="s">
+      <c r="J120" s="5">
+        <v>1</v>
+      </c>
+      <c r="K120">
+        <v>1</v>
+      </c>
+      <c r="M120" s="12" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="12" t="s">
@@ -4940,11 +5375,14 @@
       <c r="I121" s="12" t="s">
         <v>538</v>
       </c>
-      <c r="J121">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J121" s="5">
+        <v>1</v>
+      </c>
+      <c r="K121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="12" t="s">
@@ -4968,11 +5406,14 @@
       <c r="I122" s="12" t="s">
         <v>538</v>
       </c>
-      <c r="J122">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J122" s="5">
+        <v>1</v>
+      </c>
+      <c r="K122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="12" t="s">
@@ -4996,11 +5437,14 @@
       <c r="I123" s="12" t="s">
         <v>538</v>
       </c>
-      <c r="J123">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J123" s="5">
+        <v>1</v>
+      </c>
+      <c r="K123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="12" t="s">
@@ -5024,11 +5468,14 @@
       <c r="I124" s="12" t="s">
         <v>538</v>
       </c>
-      <c r="J124">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J124" s="5">
+        <v>1</v>
+      </c>
+      <c r="K124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="12" t="s">
@@ -5052,11 +5499,14 @@
       <c r="I125" s="12" t="s">
         <v>538</v>
       </c>
-      <c r="J125">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J125" s="5">
+        <v>1</v>
+      </c>
+      <c r="K125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
         <v>296</v>
       </c>
@@ -5076,11 +5526,14 @@
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
-      <c r="L126" s="10" t="s">
+      <c r="J126" s="5">
+        <v>0</v>
+      </c>
+      <c r="M126" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
         <v>299</v>
       </c>
@@ -5098,11 +5551,14 @@
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
-      <c r="L127" s="10" t="s">
+      <c r="J127" s="5">
+        <v>0</v>
+      </c>
+      <c r="M127" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
         <v>301</v>
       </c>
@@ -5120,11 +5576,14 @@
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
-      <c r="L128" s="10" t="s">
+      <c r="J128" s="5">
+        <v>0</v>
+      </c>
+      <c r="M128" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
         <v>303</v>
       </c>
@@ -5142,11 +5601,14 @@
       <c r="G129" s="3"/>
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
-      <c r="L129" s="10" t="s">
+      <c r="J129" s="5">
+        <v>0</v>
+      </c>
+      <c r="M129" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A130" s="5" t="s">
         <v>305</v>
       </c>
@@ -5164,11 +5626,14 @@
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
-      <c r="L130" s="10" t="s">
+      <c r="J130" s="5">
+        <v>0</v>
+      </c>
+      <c r="M130" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
         <v>307</v>
       </c>
@@ -5188,11 +5653,14 @@
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
-      <c r="L131" s="10" t="s">
+      <c r="J131" s="5">
+        <v>0</v>
+      </c>
+      <c r="M131" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A132" s="5" t="s">
         <v>310</v>
       </c>
@@ -5212,11 +5680,14 @@
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
-      <c r="L132" s="10" t="s">
+      <c r="J132" s="5">
+        <v>0</v>
+      </c>
+      <c r="M132" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="12" t="s">
@@ -5230,11 +5701,14 @@
       <c r="G133" s="3"/>
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
-      <c r="L133" s="10" t="s">
+      <c r="J133" s="5">
+        <v>0</v>
+      </c>
+      <c r="M133" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A134" s="5" t="s">
         <v>313</v>
       </c>
@@ -5254,11 +5728,14 @@
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
-      <c r="L134" s="10" t="s">
+      <c r="J134" s="5">
+        <v>0</v>
+      </c>
+      <c r="M134" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A135" s="5" t="s">
         <v>315</v>
       </c>
@@ -5278,11 +5755,14 @@
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
-      <c r="L135" s="10" t="s">
+      <c r="J135" s="5">
+        <v>0</v>
+      </c>
+      <c r="M135" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="12" t="s">
@@ -5296,11 +5776,14 @@
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
-      <c r="L136" s="10" t="s">
+      <c r="J136" s="5">
+        <v>0</v>
+      </c>
+      <c r="M136" s="10" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="5"/>
@@ -5312,8 +5795,11 @@
       <c r="G137" s="3"/>
       <c r="H137" s="3"/>
       <c r="I137" s="3"/>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J137" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="5"/>
@@ -5325,8 +5811,11 @@
       <c r="G138" s="3"/>
       <c r="H138" s="3"/>
       <c r="I138" s="3"/>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J138" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
         <v>321</v>
       </c>
@@ -5355,9 +5844,12 @@
       <c r="J139" s="5">
         <v>1</v>
       </c>
-      <c r="K139" s="5"/>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K139" s="5">
+        <v>1</v>
+      </c>
+      <c r="L139" s="5"/>
+    </row>
+    <row r="140" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A140" s="5" t="s">
         <v>324</v>
       </c>
@@ -5386,8 +5878,11 @@
       <c r="J140" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K140" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A141" s="5" t="s">
         <v>324</v>
       </c>
@@ -5416,8 +5911,11 @@
       <c r="J141" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K141" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
         <v>324</v>
       </c>
@@ -5446,8 +5944,11 @@
       <c r="J142" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K142" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
         <v>324</v>
       </c>
@@ -5476,8 +5977,11 @@
       <c r="J143" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K143" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A144" s="5" t="s">
         <v>324</v>
       </c>
@@ -5506,8 +6010,11 @@
       <c r="J144" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K144" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A145" s="5" t="s">
         <v>324</v>
       </c>
@@ -5536,8 +6043,11 @@
       <c r="J145" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K145" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A146" s="5" t="s">
         <v>324</v>
       </c>
@@ -5566,8 +6076,11 @@
       <c r="J146" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K146" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A147" s="5" t="s">
         <v>324</v>
       </c>
@@ -5596,8 +6109,11 @@
       <c r="J147" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K147" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A148" s="5" t="s">
         <v>350</v>
       </c>
@@ -5626,9 +6142,12 @@
       <c r="J148" s="5">
         <v>1</v>
       </c>
-      <c r="K148" s="5"/>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K148" s="5">
+        <v>1</v>
+      </c>
+      <c r="L148" s="5"/>
+    </row>
+    <row r="149" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A149" s="5" t="s">
         <v>353</v>
       </c>
@@ -5657,11 +6176,14 @@
       <c r="J149" s="5">
         <v>1</v>
       </c>
-      <c r="L149" s="5" t="s">
+      <c r="K149" s="5">
+        <v>1</v>
+      </c>
+      <c r="M149" s="5" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A150" s="5" t="s">
         <v>356</v>
       </c>
@@ -5690,11 +6212,14 @@
       <c r="J150" s="5">
         <v>1</v>
       </c>
-      <c r="L150" s="5" t="s">
+      <c r="K150" s="5">
+        <v>1</v>
+      </c>
+      <c r="M150" s="5" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A151" s="3"/>
       <c r="B151" s="3"/>
       <c r="C151" s="12" t="s">
@@ -5708,8 +6233,11 @@
       <c r="G151" s="3"/>
       <c r="H151" s="3"/>
       <c r="I151" s="3"/>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J151" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A152" s="5" t="s">
         <v>360</v>
       </c>
@@ -5738,9 +6266,12 @@
       <c r="J152" s="5">
         <v>1</v>
       </c>
-      <c r="K152" s="5"/>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K152" s="5">
+        <v>1</v>
+      </c>
+      <c r="L152" s="5"/>
+    </row>
+    <row r="153" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A153" s="5" t="s">
         <v>360</v>
       </c>
@@ -5769,9 +6300,12 @@
       <c r="J153" s="5">
         <v>1</v>
       </c>
-      <c r="K153" s="5"/>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K153" s="5">
+        <v>1</v>
+      </c>
+      <c r="L153" s="5"/>
+    </row>
+    <row r="154" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
         <v>360</v>
       </c>
@@ -5800,9 +6334,12 @@
       <c r="J154" s="5">
         <v>1</v>
       </c>
-      <c r="K154" s="5"/>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K154" s="5">
+        <v>1</v>
+      </c>
+      <c r="L154" s="5"/>
+    </row>
+    <row r="155" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A155" s="5" t="s">
         <v>360</v>
       </c>
@@ -5831,9 +6368,12 @@
       <c r="J155" s="5">
         <v>1</v>
       </c>
-      <c r="K155" s="5"/>
-    </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K155" s="5">
+        <v>1</v>
+      </c>
+      <c r="L155" s="5"/>
+    </row>
+    <row r="156" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A156" s="5" t="s">
         <v>360</v>
       </c>
@@ -5862,9 +6402,12 @@
       <c r="J156" s="5">
         <v>1</v>
       </c>
-      <c r="K156" s="5"/>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K156" s="5">
+        <v>1</v>
+      </c>
+      <c r="L156" s="5"/>
+    </row>
+    <row r="157" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A157" s="5" t="s">
         <v>360</v>
       </c>
@@ -5893,9 +6436,12 @@
       <c r="J157" s="5">
         <v>1</v>
       </c>
-      <c r="K157" s="5"/>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K157" s="5">
+        <v>1</v>
+      </c>
+      <c r="L157" s="5"/>
+    </row>
+    <row r="158" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A158" s="3"/>
       <c r="B158" s="3"/>
       <c r="C158" s="12" t="s">
@@ -5909,8 +6455,11 @@
       <c r="G158" s="3"/>
       <c r="H158" s="3"/>
       <c r="I158" s="3"/>
-    </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J158" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A159" s="5" t="s">
         <v>360</v>
       </c>
@@ -5939,9 +6488,12 @@
       <c r="J159" s="5">
         <v>1</v>
       </c>
-      <c r="K159" s="5"/>
-    </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K159" s="5">
+        <v>1</v>
+      </c>
+      <c r="L159" s="5"/>
+    </row>
+    <row r="160" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A160" s="5" t="s">
         <v>360</v>
       </c>
@@ -5970,9 +6522,12 @@
       <c r="J160" s="5">
         <v>1</v>
       </c>
-      <c r="K160" s="5"/>
-    </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K160" s="5">
+        <v>1</v>
+      </c>
+      <c r="L160" s="5"/>
+    </row>
+    <row r="161" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A161" s="3"/>
       <c r="B161" s="3"/>
       <c r="C161" s="5"/>
@@ -5984,8 +6539,11 @@
       <c r="G161" s="3"/>
       <c r="H161" s="3"/>
       <c r="I161" s="3"/>
-    </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J161" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A162" s="5" t="s">
         <v>373</v>
       </c>
@@ -6006,9 +6564,12 @@
       <c r="J162" s="5">
         <v>1</v>
       </c>
-      <c r="K162" s="5"/>
-    </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K162" s="5">
+        <v>1</v>
+      </c>
+      <c r="L162" s="5"/>
+    </row>
+    <row r="163" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A163" s="5" t="s">
         <v>377</v>
       </c>
@@ -6029,9 +6590,12 @@
       <c r="J163" s="5">
         <v>1</v>
       </c>
-      <c r="K163" s="5"/>
-    </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K163" s="5">
+        <v>1</v>
+      </c>
+      <c r="L163" s="5"/>
+    </row>
+    <row r="164" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A164" s="5" t="s">
         <v>379</v>
       </c>
@@ -6053,11 +6617,14 @@
       <c r="G164" s="3"/>
       <c r="H164" s="3"/>
       <c r="I164" s="3"/>
-      <c r="L164" t="s">
+      <c r="J164" s="5">
+        <v>1</v>
+      </c>
+      <c r="M164" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A165" s="5" t="s">
         <v>382</v>
       </c>
@@ -6084,9 +6651,12 @@
       <c r="J165" s="5">
         <v>1</v>
       </c>
-      <c r="K165" s="5"/>
-    </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K165" s="5">
+        <v>1</v>
+      </c>
+      <c r="L165" s="5"/>
+    </row>
+    <row r="166" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A166" s="5" t="s">
         <v>387</v>
       </c>
@@ -6113,9 +6683,12 @@
       <c r="J166" s="5">
         <v>1</v>
       </c>
-      <c r="K166" s="5"/>
-    </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K166" s="5">
+        <v>1</v>
+      </c>
+      <c r="L166" s="5"/>
+    </row>
+    <row r="167" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A167" s="5" t="s">
         <v>389</v>
       </c>
@@ -6142,11 +6715,14 @@
       <c r="J167" s="5">
         <v>1</v>
       </c>
-      <c r="K167" s="5" t="s">
+      <c r="K167" s="5">
+        <v>1</v>
+      </c>
+      <c r="L167" s="5" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A168" s="5" t="s">
         <v>393</v>
       </c>
@@ -6175,9 +6751,12 @@
       <c r="J168" s="5">
         <v>1</v>
       </c>
-      <c r="K168" s="5"/>
-    </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K168" s="5">
+        <v>1</v>
+      </c>
+      <c r="L168" s="5"/>
+    </row>
+    <row r="169" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A169" s="5" t="s">
         <v>397</v>
       </c>
@@ -6206,9 +6785,12 @@
       <c r="J169" s="5">
         <v>1</v>
       </c>
-      <c r="K169" s="5"/>
-    </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K169" s="5">
+        <v>1</v>
+      </c>
+      <c r="L169" s="5"/>
+    </row>
+    <row r="170" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A170" s="5" t="s">
         <v>401</v>
       </c>
@@ -6237,9 +6819,12 @@
       <c r="J170" s="5">
         <v>1</v>
       </c>
-      <c r="K170" s="5"/>
-    </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K170" s="5">
+        <v>1</v>
+      </c>
+      <c r="L170" s="5"/>
+    </row>
+    <row r="171" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A171" s="3"/>
       <c r="B171" s="3"/>
       <c r="C171" s="5"/>
@@ -6251,11 +6836,14 @@
       <c r="G171" s="3"/>
       <c r="H171" s="3"/>
       <c r="I171" s="3"/>
-      <c r="L171" t="s">
+      <c r="J171" s="5">
+        <v>1</v>
+      </c>
+      <c r="M171" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A172" s="3"/>
       <c r="B172" s="3"/>
       <c r="C172" s="5"/>
@@ -6267,8 +6855,11 @@
       <c r="G172" s="3"/>
       <c r="H172" s="3"/>
       <c r="I172" s="3"/>
-    </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J172" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A173" s="3"/>
       <c r="B173" s="3"/>
       <c r="C173" s="5"/>
@@ -6280,8 +6871,11 @@
       <c r="G173" s="3"/>
       <c r="H173" s="3"/>
       <c r="I173" s="3"/>
-    </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J173" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A174" s="3"/>
       <c r="B174" s="3"/>
       <c r="C174" s="5"/>
@@ -6293,8 +6887,11 @@
       <c r="G174" s="3"/>
       <c r="H174" s="3"/>
       <c r="I174" s="3"/>
-    </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J174" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A175" s="3"/>
       <c r="B175" s="3"/>
       <c r="C175" s="5"/>
@@ -6306,8 +6903,11 @@
       <c r="G175" s="3"/>
       <c r="H175" s="3"/>
       <c r="I175" s="3"/>
-    </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J175" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A176" s="3"/>
       <c r="B176" s="3"/>
       <c r="C176" s="5"/>
@@ -6319,8 +6919,11 @@
       <c r="G176" s="3"/>
       <c r="H176" s="3"/>
       <c r="I176" s="3"/>
-    </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J176" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A177" s="3"/>
       <c r="B177" s="3"/>
       <c r="C177" s="5"/>
@@ -6332,8 +6935,11 @@
       <c r="G177" s="3"/>
       <c r="H177" s="3"/>
       <c r="I177" s="3"/>
-    </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J177" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A178" s="3"/>
       <c r="B178" s="3"/>
       <c r="C178" s="5"/>
@@ -6345,8 +6951,11 @@
       <c r="G178" s="3"/>
       <c r="H178" s="3"/>
       <c r="I178" s="3"/>
-    </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J178" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A179" s="3"/>
       <c r="B179" s="3"/>
       <c r="C179" s="5"/>
@@ -6358,8 +6967,11 @@
       <c r="G179" s="3"/>
       <c r="H179" s="3"/>
       <c r="I179" s="3"/>
-    </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J179" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
       <c r="C180" s="5"/>
@@ -6371,8 +6983,11 @@
       <c r="G180" s="3"/>
       <c r="H180" s="3"/>
       <c r="I180" s="3"/>
-    </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J180" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A181" s="3"/>
       <c r="B181" s="3"/>
       <c r="C181" s="5"/>
@@ -6384,8 +6999,11 @@
       <c r="G181" s="3"/>
       <c r="H181" s="3"/>
       <c r="I181" s="3"/>
-    </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J181" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A182" s="3"/>
       <c r="B182" s="3"/>
       <c r="C182" s="5"/>
@@ -6397,8 +7015,11 @@
       <c r="G182" s="3"/>
       <c r="H182" s="3"/>
       <c r="I182" s="3"/>
-    </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J182" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A183" s="3"/>
       <c r="B183" s="3"/>
       <c r="C183" s="5"/>
@@ -6410,8 +7031,11 @@
       <c r="G183" s="3"/>
       <c r="H183" s="3"/>
       <c r="I183" s="3"/>
-    </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J183" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A184" s="3"/>
       <c r="B184" s="3"/>
       <c r="C184" s="5"/>
@@ -6423,8 +7047,11 @@
       <c r="G184" s="3"/>
       <c r="H184" s="3"/>
       <c r="I184" s="3"/>
-    </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J184" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A185" s="3"/>
       <c r="B185" s="3"/>
       <c r="C185" s="5"/>
@@ -6436,8 +7063,11 @@
       <c r="G185" s="3"/>
       <c r="H185" s="3"/>
       <c r="I185" s="3"/>
-    </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J185" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A186" s="3"/>
       <c r="B186" s="3"/>
       <c r="C186" s="5"/>
@@ -6449,8 +7079,11 @@
       <c r="G186" s="3"/>
       <c r="H186" s="3"/>
       <c r="I186" s="3"/>
-    </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J186" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A187" s="3"/>
       <c r="B187" s="3"/>
       <c r="C187" s="5"/>
@@ -6462,8 +7095,11 @@
       <c r="G187" s="3"/>
       <c r="H187" s="3"/>
       <c r="I187" s="3"/>
-    </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J187" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A188" s="3"/>
       <c r="B188" s="3"/>
       <c r="C188" s="5"/>
@@ -6475,8 +7111,14 @@
       <c r="G188" s="3"/>
       <c r="H188" s="3"/>
       <c r="I188" s="3"/>
-    </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J188" s="5">
+        <v>0</v>
+      </c>
+      <c r="M188" s="10" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A189" s="3"/>
       <c r="B189" s="3"/>
       <c r="C189" s="5"/>
@@ -6488,8 +7130,14 @@
       <c r="G189" s="3"/>
       <c r="H189" s="3"/>
       <c r="I189" s="3"/>
-    </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J189" s="5">
+        <v>0</v>
+      </c>
+      <c r="M189" s="10" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A190" s="3"/>
       <c r="B190" s="3"/>
       <c r="C190" s="5"/>
@@ -6501,8 +7149,14 @@
       <c r="G190" s="3"/>
       <c r="H190" s="3"/>
       <c r="I190" s="3"/>
-    </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J190" s="5">
+        <v>0</v>
+      </c>
+      <c r="M190" s="10" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A191" s="5" t="s">
         <v>423</v>
       </c>
@@ -6522,11 +7176,14 @@
       <c r="G191" s="3"/>
       <c r="H191" s="3"/>
       <c r="I191" s="3"/>
-      <c r="L191" t="s">
+      <c r="J191" s="5">
+        <v>1</v>
+      </c>
+      <c r="M191" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A192" s="5" t="s">
         <v>426</v>
       </c>
@@ -6555,23 +7212,37 @@
       <c r="J192" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="193" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K192" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="9:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="I193" s="9" t="s">
         <v>454</v>
       </c>
-      <c r="J193">
+      <c r="J193" s="9"/>
+      <c r="K193">
+        <f>SUM(K2:K192)</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="194" spans="9:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I194" s="10" t="s">
+        <v>563</v>
+      </c>
+      <c r="J194">
         <f>SUM(J2:J192)</f>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="194" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I194" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="195" spans="9:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I195" s="9" t="s">
         <v>455</v>
       </c>
-      <c r="J194" s="11">
-        <f>J193/191</f>
-        <v>0.44502617801047123</v>
+      <c r="J195" s="9"/>
+      <c r="K195" s="11">
+        <f>K193/J194</f>
+        <v>0.62130177514792895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
JarExtInspector: make knownShas a Constant property
</commit_message>
<xml_diff>
--- a/doc-project/R2019b jarext worksheet.xlsx
+++ b/doc-project/R2019b jarext worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janke/local/repos/matlab-jump/doc-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE5B727-97EA-8146-B28C-ECC36D9DCC21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB7F94D-D9FA-9C49-B71D-16DB1C1B7E10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29940" windowHeight="25360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="34520" windowHeight="21480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="R2019b" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="576">
   <si>
     <t>Title</t>
   </si>
@@ -1743,6 +1743,24 @@
   </si>
   <si>
     <t>HACK: I'm using 1.7.0 bc there never was a real 1.7.1 release.</t>
+  </si>
+  <si>
+    <t>LGPL/MPL</t>
+  </si>
+  <si>
+    <t>org.jogamp.gluegen</t>
+  </si>
+  <si>
+    <t>gluegen-rt</t>
+  </si>
+  <si>
+    <t>HACK: Matlab is using an RC; I just went with the GM version.</t>
+  </si>
+  <si>
+    <t>net.sourceforge.collections</t>
+  </si>
+  <si>
+    <t>collections-generic</t>
   </si>
 </sst>
 </file>
@@ -2076,10 +2094,10 @@
   <dimension ref="A1:M195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K75" sqref="K75"/>
+      <selection pane="bottomRight" activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3550,9 +3568,15 @@
         <v>136</v>
       </c>
       <c r="F50" s="5"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
+      <c r="G50" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="I50" s="3">
+        <v>4.01</v>
+      </c>
       <c r="J50" s="5">
         <v>1</v>
       </c>
@@ -4138,7 +4162,9 @@
         <v>187</v>
       </c>
       <c r="B74" s="3"/>
-      <c r="C74" s="5"/>
+      <c r="C74" s="5" t="s">
+        <v>570</v>
+      </c>
       <c r="D74" s="6" t="s">
         <v>188</v>
       </c>
@@ -4180,11 +4206,23 @@
         <v>193</v>
       </c>
       <c r="F75" s="5"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
+      <c r="G75" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>523</v>
+      </c>
       <c r="J75" s="5">
         <v>1</v>
+      </c>
+      <c r="K75">
+        <v>1</v>
+      </c>
+      <c r="M75" s="10" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -7247,7 +7285,7 @@
       <c r="J193" s="9"/>
       <c r="K193">
         <f>SUM(K2:K192)</f>
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="194" spans="9:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7266,7 +7304,7 @@
       <c r="J195" s="9"/>
       <c r="K195" s="11">
         <f>K193/J194</f>
-        <v>0.62721893491124259</v>
+        <v>0.63313609467455623</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix filenames for JSch distribution JARs
</commit_message>
<xml_diff>
--- a/doc-project/R2019b jarext worksheet.xlsx
+++ b/doc-project/R2019b jarext worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janke/local/repos/matlab-jump/doc-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB7F94D-D9FA-9C49-B71D-16DB1C1B7E10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4C9BAF-866F-2D4E-821B-BE005FD8605C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="34520" windowHeight="21480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2094,10 +2094,10 @@
   <dimension ref="A1:M195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B157" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J50" sqref="J50"/>
+      <selection pane="bottomRight" activeCell="M119" sqref="M119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Note about tablelayout.jar in worksheet
</commit_message>
<xml_diff>
--- a/doc-project/R2019b jarext worksheet.xlsx
+++ b/doc-project/R2019b jarext worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janke/local/repos/matlab-jump/doc-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4C9BAF-866F-2D4E-821B-BE005FD8605C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BCAD75-1B62-B04F-A74B-88BF4227F0D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="34520" windowHeight="21480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="578">
   <si>
     <t>Title</t>
   </si>
@@ -1761,6 +1761,12 @@
   </si>
   <si>
     <t>collections-generic</t>
+  </si>
+  <si>
+    <t>c385ac80a618abc53952b3e6b1967edd5bfcb0a6daa10a9ed8858d8a8317b909</t>
+  </si>
+  <si>
+    <t>Couldn't find this anywhere. Asked MathWorks.</t>
   </si>
 </sst>
 </file>
@@ -2094,10 +2100,10 @@
   <dimension ref="A1:M195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B157" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B141" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M119" sqref="M119"/>
+      <selection pane="bottomRight" activeCell="M173" sqref="M173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6914,11 +6920,16 @@
         <v>404</v>
       </c>
       <c r="F172" s="5"/>
-      <c r="G172" s="3"/>
+      <c r="G172" s="3" t="s">
+        <v>576</v>
+      </c>
       <c r="H172" s="3"/>
       <c r="I172" s="3"/>
       <c r="J172" s="5">
         <v>1</v>
+      </c>
+      <c r="M172" s="10" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="173" spans="1:13" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
R2019b: add antlr dep
</commit_message>
<xml_diff>
--- a/doc-project/R2019b jarext worksheet.xlsx
+++ b/doc-project/R2019b jarext worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janke/local/repos/matlab-jump/doc-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BCAD75-1B62-B04F-A74B-88BF4227F0D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04509AFE-FAAB-1449-BAD5-85D0115B96ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="34520" windowHeight="21480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1685,9 +1685,6 @@
     <t>BSD</t>
   </si>
   <si>
-    <t>SHA doesn't match any 3.x or 4.x JARs from the ANTLR website. I've asked MathWorks what this is.</t>
-  </si>
-  <si>
     <t>Apache 2.0, BSD 2-Clause</t>
   </si>
   <si>
@@ -1767,6 +1764,9 @@
   </si>
   <si>
     <t>Couldn't find this anywhere. Asked MathWorks.</t>
+  </si>
+  <si>
+    <t>SHA doesn't match any 3.x or 4.x JARs from the ANTLR website. Determined version by running "java -jar antlr.jar", which prints the help screen including version info.</t>
   </si>
 </sst>
 </file>
@@ -2100,10 +2100,10 @@
   <dimension ref="A1:M195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B141" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M173" sqref="M173"/>
+      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2150,7 +2150,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>429</v>
@@ -2191,7 +2191,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D3" s="6">
         <v>1</v>
@@ -2291,7 +2291,9 @@
       <c r="C8" s="12" t="s">
         <v>530</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4">
+        <v>3.3</v>
+      </c>
       <c r="E8" s="5" t="s">
         <v>16</v>
       </c>
@@ -2304,8 +2306,11 @@
       <c r="J8" s="5">
         <v>1</v>
       </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
       <c r="M8" s="10" t="s">
-        <v>550</v>
+        <v>577</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -2451,7 +2456,7 @@
         <v>31</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D14" s="6">
         <v>1.1000000000000001</v>
@@ -2782,7 +2787,7 @@
         <v>31</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D24" s="6">
         <v>1.4</v>
@@ -2849,7 +2854,7 @@
         <v>77</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D26" s="6">
         <v>1.6</v>
@@ -3575,10 +3580,10 @@
       </c>
       <c r="F50" s="5"/>
       <c r="G50" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="H50" s="3" t="s">
         <v>574</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>575</v>
       </c>
       <c r="I50" s="3">
         <v>4.01</v>
@@ -3958,7 +3963,7 @@
         <v>168</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>169</v>
@@ -4169,7 +4174,7 @@
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>188</v>
@@ -4179,22 +4184,22 @@
       </c>
       <c r="F74" s="5"/>
       <c r="G74" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="H74" s="3" t="s">
         <v>566</v>
       </c>
-      <c r="H74" s="3" t="s">
+      <c r="I74" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="I74" s="3" t="s">
+      <c r="J74" s="5">
+        <v>1</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+      <c r="M74" s="10" t="s">
         <v>568</v>
-      </c>
-      <c r="J74" s="5">
-        <v>1</v>
-      </c>
-      <c r="K74">
-        <v>1</v>
-      </c>
-      <c r="M74" s="10" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -4213,10 +4218,10 @@
       </c>
       <c r="F75" s="5"/>
       <c r="G75" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="H75" s="3" t="s">
         <v>571</v>
-      </c>
-      <c r="H75" s="3" t="s">
-        <v>572</v>
       </c>
       <c r="I75" s="3" t="s">
         <v>523</v>
@@ -4228,7 +4233,7 @@
         <v>1</v>
       </c>
       <c r="M75" s="10" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -4872,7 +4877,7 @@
         <v>255</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>35</v>
@@ -4925,7 +4930,7 @@
         <v>259</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D103" s="6">
         <v>1</v>
@@ -4959,7 +4964,7 @@
         <v>262</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>263</v>
@@ -4993,7 +4998,7 @@
         <v>262</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>263</v>
@@ -5072,7 +5077,7 @@
         <v>275</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>276</v>
@@ -5097,7 +5102,7 @@
         <v>275</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>276</v>
@@ -5120,7 +5125,7 @@
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="12" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D110" s="13"/>
       <c r="E110" s="5" t="s">
@@ -5140,7 +5145,7 @@
         <v>275</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D111" s="13" t="s">
         <v>276</v>
@@ -5165,7 +5170,7 @@
         <v>275</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>276</v>
@@ -5190,7 +5195,7 @@
         <v>275</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>276</v>
@@ -5215,7 +5220,7 @@
         <v>275</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>276</v>
@@ -5238,7 +5243,7 @@
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="5" t="s">
@@ -5261,7 +5266,7 @@
         <v>275</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>276</v>
@@ -5582,7 +5587,7 @@
         <v>297</v>
       </c>
       <c r="C126" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D126" s="6">
         <v>2.1</v>
@@ -5609,7 +5614,7 @@
         <v>297</v>
       </c>
       <c r="C127" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="5" t="s">
@@ -5634,7 +5639,7 @@
         <v>297</v>
       </c>
       <c r="C128" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D128" s="4"/>
       <c r="E128" s="5" t="s">
@@ -5659,7 +5664,7 @@
         <v>297</v>
       </c>
       <c r="C129" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D129" s="4"/>
       <c r="E129" s="5" t="s">
@@ -5684,7 +5689,7 @@
         <v>297</v>
       </c>
       <c r="C130" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="5" t="s">
@@ -5709,7 +5714,7 @@
         <v>297</v>
       </c>
       <c r="C131" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D131" s="6" t="s">
         <v>308</v>
@@ -5736,7 +5741,7 @@
         <v>297</v>
       </c>
       <c r="C132" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D132" s="6">
         <v>3.3</v>
@@ -5759,7 +5764,7 @@
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="5" t="s">
@@ -5784,7 +5789,7 @@
         <v>297</v>
       </c>
       <c r="C134" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D134" s="6" t="s">
         <v>308</v>
@@ -5811,7 +5816,7 @@
         <v>297</v>
       </c>
       <c r="C135" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D135" s="6" t="s">
         <v>316</v>
@@ -5834,7 +5839,7 @@
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D136" s="4"/>
       <c r="E136" s="5" t="s">
@@ -6291,7 +6296,7 @@
       <c r="A151" s="3"/>
       <c r="B151" s="3"/>
       <c r="C151" s="12" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D151" s="4"/>
       <c r="E151" s="5" t="s">
@@ -6313,7 +6318,7 @@
         <v>361</v>
       </c>
       <c r="C152" s="12" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D152" s="6" t="s">
         <v>362</v>
@@ -6347,7 +6352,7 @@
         <v>361</v>
       </c>
       <c r="C153" s="12" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D153" s="6" t="s">
         <v>362</v>
@@ -6381,7 +6386,7 @@
         <v>361</v>
       </c>
       <c r="C154" s="12" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D154" s="6" t="s">
         <v>362</v>
@@ -6415,7 +6420,7 @@
         <v>361</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D155" s="6" t="s">
         <v>362</v>
@@ -6449,7 +6454,7 @@
         <v>361</v>
       </c>
       <c r="C156" s="12" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D156" s="6" t="s">
         <v>362</v>
@@ -6483,7 +6488,7 @@
         <v>361</v>
       </c>
       <c r="C157" s="12" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D157" s="6" t="s">
         <v>362</v>
@@ -6513,7 +6518,7 @@
       <c r="A158" s="3"/>
       <c r="B158" s="3"/>
       <c r="C158" s="12" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D158" s="4"/>
       <c r="E158" s="5" t="s">
@@ -6535,7 +6540,7 @@
         <v>361</v>
       </c>
       <c r="C159" s="12" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D159" s="6" t="s">
         <v>362</v>
@@ -6569,7 +6574,7 @@
         <v>361</v>
       </c>
       <c r="C160" s="12" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D160" s="6" t="s">
         <v>362</v>
@@ -6798,7 +6803,7 @@
         <v>394</v>
       </c>
       <c r="C168" s="12" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D168" s="6" t="s">
         <v>395</v>
@@ -6832,7 +6837,7 @@
         <v>398</v>
       </c>
       <c r="C169" s="12" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D169" s="6" t="s">
         <v>399</v>
@@ -6866,7 +6871,7 @@
         <v>398</v>
       </c>
       <c r="C170" s="12" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D170" s="6" t="s">
         <v>399</v>
@@ -6921,7 +6926,7 @@
       </c>
       <c r="F172" s="5"/>
       <c r="G172" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H172" s="3"/>
       <c r="I172" s="3"/>
@@ -6929,7 +6934,7 @@
         <v>1</v>
       </c>
       <c r="M172" s="10" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="173" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -7188,7 +7193,7 @@
         <v>0</v>
       </c>
       <c r="M188" s="10" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="189" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -7207,7 +7212,7 @@
         <v>0</v>
       </c>
       <c r="M189" s="10" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="190" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -7226,7 +7231,7 @@
         <v>0</v>
       </c>
       <c r="M190" s="10" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="191" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -7296,12 +7301,12 @@
       <c r="J193" s="9"/>
       <c r="K193">
         <f>SUM(K2:K192)</f>
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="194" spans="9:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="I194" s="10" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="J194">
         <f>SUM(J2:J192)</f>
@@ -7315,7 +7320,7 @@
       <c r="J195" s="9"/>
       <c r="K195" s="11">
         <f>K193/J194</f>
-        <v>0.63313609467455623</v>
+        <v>0.63905325443786987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>